<commit_message>
Migrate validation to pandera
* Simplify schema validation and transformation by moving from great
expectations to pandera.
* Extract most of the code out of the solids in separate modules
* Increase test coverage
</commit_message>
<xml_diff>
--- a/files/valid.xlsx
+++ b/files/valid.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\docker-desktop-data\version-pack-data\community\docker\volumes\dev-workspace\_data\dev\dealpipe\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{994D691C-98C2-4148-843B-4393B5D0D1F5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED2B8D7C-E9E0-4527-AE8A-E1AAF4E5DBC1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6620" yWindow="3230" windowWidth="28800" windowHeight="15910" xr2:uid="{86C814FD-B144-40F2-A4AD-715DE6C4DF29}"/>
+    <workbookView xWindow="5990" yWindow="1880" windowWidth="28800" windowHeight="15910" xr2:uid="{86C814FD-B144-40F2-A4AD-715DE6C4DF29}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="30">
   <si>
     <t>D1</t>
   </si>
@@ -100,15 +100,9 @@
     <t>Glass</t>
   </si>
   <si>
-    <t>yes</t>
-  </si>
-  <si>
     <t>Airbus A320</t>
   </si>
   <si>
-    <t>no</t>
-  </si>
-  <si>
     <t>DealName</t>
   </si>
   <si>
@@ -128,6 +122,9 @@
   </si>
   <si>
     <t>Countries</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -482,7 +479,7 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -496,7 +493,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -514,16 +511,16 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" t="s">
         <v>25</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>26</v>
-      </c>
-      <c r="I1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
@@ -607,7 +604,7 @@
         <v>11.2</v>
       </c>
       <c r="G4" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="H4" t="s">
         <v>7</v>
@@ -621,13 +618,13 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B5">
         <v>22219387192.129299</v>
       </c>
       <c r="G5" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="H5" t="s">
         <v>17</v>
@@ -661,16 +658,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C1" t="s">
         <v>14</v>
       </c>
       <c r="D1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">

</xml_diff>